<commit_message>
Actualizacion y nuevos elementos
Registro Banco y Movimiento, nuevas variables, actualizacion de base de datos y la informacion agregada al Read Me
</commit_message>
<xml_diff>
--- a/Entregables/Carga Masiva REM y ejemplo.xlsx
+++ b/Entregables/Carga Masiva REM y ejemplo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Aplicacion\Entregables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lilian\Documents\GitHub\FinTech\Entregables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B42B0B21-5C2D-4ED7-9F1B-4789954AC3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE626B19-636F-4EC5-A5AF-DB0F82B36341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{D305AF94-B9ED-4F11-8162-16502303EC1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{D305AF94-B9ED-4F11-8162-16502303EC1F}"/>
   </bookViews>
   <sheets>
     <sheet name="ABRIL 2023" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
   <si>
     <t>DTH CONSULTORES LIMITADA</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>JOSE MANUEL ZILLERUELO MORENO</t>
-  </si>
-  <si>
-    <t>LIBRO DE REMUNERACIONES</t>
   </si>
   <si>
     <t xml:space="preserve">MES : ABRIL DEL 2023 </t>
@@ -709,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C411676-B81B-4CB7-B0CC-9D071AC64761}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -782,7 +779,7 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -811,7 +808,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -867,91 +864,91 @@
     </row>
     <row r="9" spans="1:29" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="Q9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="R9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="S9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S9" s="2" t="s">
+      <c r="T9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="U9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="V9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="V9" s="2" t="s">
+      <c r="W9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="X9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="X9" s="2" t="s">
+      <c r="Y9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Y9" s="3" t="s">
+      <c r="Z9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Z9" s="4" t="s">
+      <c r="AA9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AA9" s="4" t="s">
+      <c r="AB9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AB9" s="4" t="s">
+      <c r="AC9" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -959,16 +956,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="7">
         <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="F10" s="7">
         <v>30</v>
@@ -1049,16 +1046,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="7">
         <v>7</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="F11" s="7">
         <v>30</v>
@@ -1139,16 +1136,16 @@
         <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="7">
         <v>11</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="F12" s="7">
         <v>30</v>
@@ -1229,16 +1226,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7">
         <v>2</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="F13" s="7">
         <v>30</v>
@@ -1319,16 +1316,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="7">
         <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="F14" s="7">
         <v>30</v>
@@ -1409,16 +1406,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="7">
         <v>13</v>
       </c>
       <c r="D15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="F15" s="7">
         <v>30</v>
@@ -1499,16 +1496,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="7">
         <v>4</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="F16" s="7">
         <v>30</v>
@@ -1589,16 +1586,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="7">
         <v>10</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="F17" s="7">
         <v>30</v>
@@ -1679,16 +1676,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="7">
         <v>5</v>
       </c>
       <c r="D18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="F18" s="7">
         <v>30</v>
@@ -1766,7 +1763,7 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="E19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19" s="12">
         <v>270</v>
@@ -1864,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6512326C-AB29-4ADC-8A5A-E3709ED7EB59}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,7 +1889,7 @@
     <col min="20" max="20" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3.140625" bestFit="1" customWidth="1"/>
@@ -1903,91 +1900,91 @@
   <sheetData>
     <row r="1" spans="1:29" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -1995,88 +1992,89 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" t="s">
-        <v>59</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
-      <c r="Y2">
-        <v>1</v>
-      </c>
-      <c r="Z2">
-        <v>1</v>
-      </c>
-      <c r="AA2">
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <v>1</v>
-      </c>
-      <c r="AC2">
-        <v>1</v>
+      <c r="G2" s="9">
+        <v>1595993</v>
+      </c>
+      <c r="H2" s="9">
+        <v>162292</v>
+      </c>
+      <c r="I2" s="9">
+        <v>1758285</v>
+      </c>
+      <c r="J2" s="9">
+        <v>1758285</v>
+      </c>
+      <c r="K2" s="9">
+        <v>0</v>
+      </c>
+      <c r="L2" s="9">
+        <v>0</v>
+      </c>
+      <c r="M2" s="9">
+        <v>100000</v>
+      </c>
+      <c r="N2" s="9">
+        <v>100000</v>
+      </c>
+      <c r="O2" s="9">
+        <v>200000</v>
+      </c>
+      <c r="P2" s="9">
+        <v>1958285</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>201148</v>
+      </c>
+      <c r="R2" s="9">
+        <v>123080</v>
+      </c>
+      <c r="S2" s="9">
+        <v>23251</v>
+      </c>
+      <c r="T2" s="9">
+        <v>10550</v>
+      </c>
+      <c r="U2" s="9">
+        <v>0</v>
+      </c>
+      <c r="V2" s="9">
+        <v>358029</v>
+      </c>
+      <c r="W2" s="9">
+        <v>42705</v>
+      </c>
+      <c r="X2" s="9">
+        <v>400734</v>
+      </c>
+      <c r="Y2" s="10">
+        <v>1557551</v>
+      </c>
+      <c r="Z2" s="11">
+        <v>28308</v>
+      </c>
+      <c r="AA2" s="11">
+        <v>42199</v>
+      </c>
+      <c r="AB2" s="11">
+        <v>16352</v>
+      </c>
+      <c r="AC2" s="11">
+        <f>+P2+Z2+AA2+AB2</f>
+        <v>2045144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>